<commit_message>
Statistics task. 1.2 added title
</commit_message>
<xml_diff>
--- a/src/main/java/resources/statistic.xlsx
+++ b/src/main/java/resources/statistic.xlsx
@@ -12,21 +12,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Avg Scores</t>
+  </si>
+  <si>
+    <t>Students Number</t>
+  </si>
+  <si>
+    <t>University Number</t>
+  </si>
+  <si>
+    <t>University List</t>
+  </si>
   <si>
     <t>Физика</t>
   </si>
   <si>
+    <t>4.537499964237213</t>
+  </si>
+  <si>
     <t>МВУ, МПИ</t>
   </si>
   <si>
     <t>Медицина</t>
   </si>
   <si>
+    <t>4.333333492279053</t>
+  </si>
+  <si>
     <t>МГМУ, ТУМ, СМИ</t>
   </si>
   <si>
     <t>Лингвистика</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
   <si>
     <t>ВЛПУ</t>
@@ -80,18 +104,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:F5"/>
+  <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
+    <row r="1">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4.537499964237213</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
       <c r="D2" t="n">
         <v>8.0</v>
@@ -100,15 +141,15 @@
         <v>2.0</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4.333333492279053</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="n">
         <v>3.0</v>
@@ -117,15 +158,15 @@
         <v>3.0</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="e">
-        <v>#NUM!</v>
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
       <c r="D4" t="n">
         <v>0.0</v>
@@ -134,15 +175,15 @@
         <v>1.0</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="e">
-        <v>#NUM!</v>
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
@@ -151,7 +192,7 @@
         <v>1.0</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>